<commit_message>
unit tests + colC
</commit_message>
<xml_diff>
--- a/inst/template.xlsx
+++ b/inst/template.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -23,13 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t xml:space="preserve">Template page – to be updated. If you have any problems with the “LStest” package please see:
-Github link </t>
-  </si>
-  <si>
-    <t xml:space="preserve">email address</t>
+    <t xml:space="preserve">This is the template sheet for the package LStest – if you do not want to see this…</t>
   </si>
 </sst>
 </file>
@@ -153,29 +149,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="true"/>
   </sheetPr>
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B16" activeCellId="0" sqref="B16"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="1" width="9.13"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="27.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="27.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -186,6 +185,9 @@
     <row r="50" customFormat="false" ht="26.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="51" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:I1"/>
+  </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="0.609722222222222" bottom="1" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>